<commit_message>
Implemented multiple character phonems.
</commit_message>
<xml_diff>
--- a/res/rasgos.xlsx
+++ b/res/rasgos.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="vocales" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="vocales viejo" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="consonantes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="vocales" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="80">
   <si>
     <t xml:space="preserve">i</t>
   </si>
@@ -177,14 +178,99 @@
   </si>
   <si>
     <t xml:space="preserve">DORSAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O~</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cerrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abierta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laxa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">±</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redondeada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nasal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alargada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -252,7 +338,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +352,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,10 +379,10 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="5.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
@@ -524,11 +614,11 @@
   </sheetPr>
   <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="2" style="1" width="4.97"/>
@@ -1433,4 +1523,790 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AE8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="12" style="0" width="5.7"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>